<commit_message>
"Added new with dp."
</commit_message>
<xml_diff>
--- a/lc/lc_report.xlsx
+++ b/lc/lc_report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clair/dev/coding/PractiseCoding/lc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F0527D-ACA4-4A43-8BC3-A6FE1FE05FF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07631140-EAED-7D4B-B556-17ACF34948AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17700" yWindow="-17120" windowWidth="28800" windowHeight="16540" xr2:uid="{E41591E5-CCD4-4540-8BB6-AAC43D66D3F8}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>if list has None element, list.extend(list) will be [None]</t>
+  </si>
+  <si>
+    <t>dp</t>
+  </si>
+  <si>
+    <t>recursion</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,6 +739,21 @@
       </c>
       <c r="C10" t="s">
         <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Reviewed dfs: inorder, postorder, preorder."
</commit_message>
<xml_diff>
--- a/lc/lc_report.xlsx
+++ b/lc/lc_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clair/dev/coding/PractiseCoding/lc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07631140-EAED-7D4B-B556-17ACF34948AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA88F065-9E6B-BB44-A160-F75518C0FAC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17700" yWindow="-17120" windowWidth="28800" windowHeight="16540" xr2:uid="{E41591E5-CCD4-4540-8BB6-AAC43D66D3F8}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>recursion</t>
+  </si>
+  <si>
+    <t>positions of large group</t>
   </si>
 </sst>
 </file>
@@ -500,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8DD2BA-D9CE-C74F-B867-C2CFA462735B}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,6 +757,23 @@
       </c>
       <c r="H10">
         <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"Added new and updated report."
</commit_message>
<xml_diff>
--- a/lc/lc_report.xlsx
+++ b/lc/lc_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clair\dev\PractiseCoding\lc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clair/dev/coding/PractiseCoding/lc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89381134-8403-4421-9EB4-418D67706A4B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C49522-537C-3148-B4A0-2C7A26E257EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="2940" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{E41591E5-CCD4-4540-8BB6-AAC43D66D3F8}"/>
+    <workbookView xWindow="3500" yWindow="2940" windowWidth="21600" windowHeight="11380" xr2:uid="{E41591E5-CCD4-4540-8BB6-AAC43D66D3F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -212,6 +212,12 @@
   <si>
     <t>def postorder( r ): return postorder(r.left) + postorder(r.right) + [r.val]</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>house robber 3</t>
+  </si>
+  <si>
+    <t>d&amp;c</t>
   </si>
 </sst>
 </file>
@@ -222,13 +228,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -637,18 +643,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8DD2BA-D9CE-C74F-B867-C2CFA462735B}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -677,7 +683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -706,7 +712,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -732,7 +738,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -755,7 +761,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -778,7 +784,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -804,7 +810,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -824,7 +830,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -847,7 +853,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -867,7 +873,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -893,7 +899,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -910,7 +916,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -937,6 +943,29 @@
       </c>
       <c r="I12" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -949,18 +978,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E77D5FD-08ED-4750-8EDA-AFB321EB3791}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -971,7 +1000,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -982,7 +1011,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1008,12 +1037,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1021,7 +1050,7 @@
         <v>4.3750000000000004E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1043,9 +1072,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1064,12 +1093,12 @@
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>

</xml_diff>